<commit_message>
run latest mex files.  update qa checks on segments, drugs, bacteria.
</commit_message>
<xml_diff>
--- a/data/coded_segments/zm_3_4.xlsx
+++ b/data/coded_segments/zm_3_4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/amr-db/data/coded_segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC53F39C-9FAC-F449-87B9-FA3B701B0020}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C62606A0-7BEB-6342-9E4C-5BB1DA67A91C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2567" uniqueCount="812">
   <si>
     <t>Color</t>
   </si>
@@ -2485,6 +2485,69 @@
   </si>
   <si>
     <t>2009</t>
+  </si>
+  <si>
+    <t>1: 1640</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>11/14/18 09:53:00</t>
+  </si>
+  <si>
+    <t>1: 1653</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>11/14/18 09:54:00</t>
+  </si>
+  <si>
+    <t>1: 3610</t>
+  </si>
+  <si>
+    <t>1: 3613</t>
+  </si>
+  <si>
+    <t>11/14/18 09:55:00</t>
+  </si>
+  <si>
+    <t>1: 3671</t>
+  </si>
+  <si>
+    <t>1: 3672</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>1: 3703</t>
+  </si>
+  <si>
+    <t>1: 3727</t>
+  </si>
+  <si>
+    <t>chronic pulmonary disease</t>
+  </si>
+  <si>
+    <t>11/14/18 09:56:00</t>
+  </si>
+  <si>
+    <t>11/14/18 09:57:00</t>
+  </si>
+  <si>
+    <t>3: 519</t>
+  </si>
+  <si>
+    <t>3: 530</t>
+  </si>
+  <si>
+    <t>M. europaeum</t>
+  </si>
+  <si>
+    <t>11/14/18 09:58:00</t>
   </si>
 </sst>
 </file>
@@ -3224,7 +3287,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M243"/>
+  <dimension ref="A1:M257"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -13191,6 +13254,580 @@
         <v>787</v>
       </c>
     </row>
+    <row r="244" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A244" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="G244" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="H244" s="3">
+        <v>0</v>
+      </c>
+      <c r="I244" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="J244" s="3">
+        <v>2</v>
+      </c>
+      <c r="K244" s="4">
+        <v>1.5199000000000001E-2</v>
+      </c>
+      <c r="L244" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M244" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A245" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="G245" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="H245" s="3">
+        <v>0</v>
+      </c>
+      <c r="I245" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="J245" s="3">
+        <v>3</v>
+      </c>
+      <c r="K245" s="4">
+        <v>2.2797999999999999E-2</v>
+      </c>
+      <c r="L245" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M245" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A246" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="G246" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="H246" s="3">
+        <v>0</v>
+      </c>
+      <c r="I246" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="J246" s="3">
+        <v>3</v>
+      </c>
+      <c r="K246" s="4">
+        <v>2.2797999999999999E-2</v>
+      </c>
+      <c r="L246" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M246" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A247" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="G247" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="H247" s="3">
+        <v>0</v>
+      </c>
+      <c r="I247" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="J247" s="3">
+        <v>16</v>
+      </c>
+      <c r="K247" s="4">
+        <v>0.12159</v>
+      </c>
+      <c r="L247" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M247" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A248" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="G248" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="H248" s="3">
+        <v>0</v>
+      </c>
+      <c r="I248" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="J248" s="3">
+        <v>5</v>
+      </c>
+      <c r="K248" s="4">
+        <v>3.7997000000000003E-2</v>
+      </c>
+      <c r="L248" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M248" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A249" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="G249" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="H249" s="3">
+        <v>0</v>
+      </c>
+      <c r="I249" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="J249" s="3">
+        <v>4</v>
+      </c>
+      <c r="K249" s="4">
+        <v>3.0397E-2</v>
+      </c>
+      <c r="L249" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M249" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A250" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="G250" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="H250" s="3">
+        <v>0</v>
+      </c>
+      <c r="I250" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="J250" s="3">
+        <v>4</v>
+      </c>
+      <c r="K250" s="4">
+        <v>3.0397E-2</v>
+      </c>
+      <c r="L250" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M250" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A251" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="G251" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="H251" s="3">
+        <v>0</v>
+      </c>
+      <c r="I251" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="J251" s="3">
+        <v>2</v>
+      </c>
+      <c r="K251" s="4">
+        <v>1.5199000000000001E-2</v>
+      </c>
+      <c r="L251" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M251" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A252" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="G252" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="H252" s="3">
+        <v>0</v>
+      </c>
+      <c r="I252" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="J252" s="3">
+        <v>2</v>
+      </c>
+      <c r="K252" s="4">
+        <v>1.5199000000000001E-2</v>
+      </c>
+      <c r="L252" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M252" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A253" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="G253" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="H253" s="3">
+        <v>0</v>
+      </c>
+      <c r="I253" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="J253" s="3">
+        <v>25</v>
+      </c>
+      <c r="K253" s="4">
+        <v>0.18998399999999999</v>
+      </c>
+      <c r="L253" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M253" s="1" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A254" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="G254" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="H254" s="3">
+        <v>0</v>
+      </c>
+      <c r="I254" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="J254" s="3">
+        <v>25</v>
+      </c>
+      <c r="K254" s="4">
+        <v>0.18998399999999999</v>
+      </c>
+      <c r="L254" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M254" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A255" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="G255" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="H255" s="3">
+        <v>0</v>
+      </c>
+      <c r="I255" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="J255" s="3">
+        <v>12</v>
+      </c>
+      <c r="K255" s="4">
+        <v>9.1191999999999995E-2</v>
+      </c>
+      <c r="L255" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M255" s="1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A256" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="G256" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="H256" s="3">
+        <v>0</v>
+      </c>
+      <c r="I256" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="J256" s="3">
+        <v>12</v>
+      </c>
+      <c r="K256" s="4">
+        <v>9.1191999999999995E-2</v>
+      </c>
+      <c r="L256" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M256" s="1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A257" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="G257" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="H257" s="3">
+        <v>0</v>
+      </c>
+      <c r="I257" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="J257" s="3">
+        <v>12</v>
+      </c>
+      <c r="K257" s="4">
+        <v>9.1191999999999995E-2</v>
+      </c>
+      <c r="L257" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M257" s="1" t="s">
+        <v>811</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>